<commit_message>
Thurs. 6/4/20 21:30 updates
</commit_message>
<xml_diff>
--- a/data/Boston Marathon Stats.xlsx
+++ b/data/Boston Marathon Stats.xlsx
@@ -5,19 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erinm\Documents\Anderson_Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erinm\Documents\nss-capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2FA135-73D0-4D3E-B830-69CD324FA700}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B915C49-6A2A-42E4-9665-9D8CF4D4BB5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10968" yWindow="1086" windowWidth="9120" windowHeight="10704" firstSheet="2" activeTab="3" xr2:uid="{257F4783-A47D-4BC1-9B06-D93D190DED11}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{257F4783-A47D-4BC1-9B06-D93D190DED11}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bos Entrants&amp;Finishers" sheetId="1" r:id="rId1"/>
-    <sheet name="Bos Qualifying Cutoff History" sheetId="2" r:id="rId2"/>
-    <sheet name="Bos Qualifying Times" sheetId="3" r:id="rId3"/>
-    <sheet name="BQs_over_time" sheetId="5" r:id="rId4"/>
+    <sheet name="Bos_Age_Groups (2)" sheetId="8" r:id="rId1"/>
+    <sheet name="Bos Entrants&amp;Finishers" sheetId="1" r:id="rId2"/>
+    <sheet name="Bos Qualifying Cutoff History" sheetId="2" r:id="rId3"/>
+    <sheet name="Bos Qualifying Times" sheetId="3" r:id="rId4"/>
+    <sheet name="Bos_Age_Group_Placement_Formula" sheetId="6" r:id="rId5"/>
+    <sheet name="BQs_over_time" sheetId="5" r:id="rId6"/>
+    <sheet name="Bos_Age_Groups" sheetId="7" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="107">
   <si>
     <t>YEAR</t>
   </si>
@@ -413,6 +419,9 @@
   <si>
     <t>AG Ref No.</t>
   </si>
+  <si>
+    <t>Age Group Formula</t>
+  </si>
 </sst>
 </file>
 
@@ -530,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -538,11 +547,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -621,6 +639,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,15 +651,285 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="58">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -646,7 +937,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -21073,127 +21363,455 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="AG% of 1st in AG"/>
+      <sheetName val="bos_09_AG"/>
+      <sheetName val="Bos_Age_Groups"/>
+      <sheetName val="Road Weights"/>
+      <sheetName val="boston_marathon_results_2009 "/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="A3">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>11</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F0BBD01-FBED-4417-A64E-216A3B1D2B76}" name="Table1" displayName="Table1" ref="A4:G53" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
-  <autoFilter ref="A4:G53" xr:uid="{3F6DDC19-D566-4BC4-965F-870509961C56}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BCD665A8-DC48-4371-BEC9-85E36B63290A}" name="YEAR" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{06798F71-F324-43C3-8BA2-6CE198AE158F}" name="TOTAL ENTRANTS" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{2296CF0F-522F-4A8B-B331-2AA39E601128}" name="TOTAL ENTRANTS: MEN" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{5F300890-7957-4BA9-9943-73007F1A1C4F}" name="TOTAL ENTRANTS: WOMEN" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{92948D5C-4BB1-43D5-A11D-C418A80F5517}" name="TOTAL FINISHERS" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{BAF4C57E-65CB-47A9-A209-66F6AC1AAF88}" name="TOTAL FINISHERS: MEN" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{59C23AF6-67B2-4BC8-A5FD-176ED3F381F6}" name="TOTAL FINISHERS: WOMEN" dataDxfId="37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{E159EF23-831D-4FC2-8F03-E044834D9DCC}" name="Table415" displayName="Table415" ref="E2:F13" totalsRowShown="0">
+  <autoFilter ref="E2:F13" xr:uid="{8DCFB31A-B430-423E-82DC-9A790220481D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{56A22B84-1E40-4802-8182-BDAFAD9299B3}" name="AG Ref No."/>
+    <tableColumn id="2" xr3:uid="{5F14DF79-E235-452E-B97D-B6DC0E27AF42}" name="Age Group"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{945CDC40-C170-4D74-BF4F-2A501FDC2EE5}" name="Table81011" displayName="Table81011" ref="AG4:AJ253" totalsRowShown="0">
-  <autoFilter ref="AG4:AJ253" xr:uid="{0D6CC08B-E199-4CA5-92C7-B34C714671A0}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B3D04435-650B-45FD-A98E-E0EC10C3547E}" name="Age"/>
-    <tableColumn id="6" xr3:uid="{18C002B2-A54A-4967-B8BC-024E0ED82E13}" name="Year" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{AA207F6A-07E3-4A95-B636-24C8CCC8B945}" name="Men">
-      <calculatedColumnFormula>Table6[[#This Row],[Men]]+$S$1</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{9B32EE09-A5B9-4DC3-95D8-2349E4A40D6E}" name="Women">
-      <calculatedColumnFormula>Table6[[#This Row],[Women]]+$S$1</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C47162FF-5668-4B36-A460-2609D44826EC}" name="Table11" displayName="Table11" ref="A1:E250" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E250" xr:uid="{512EA7CA-480E-423A-92C9-18C2E1562366}"/>
-  <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{312D51B1-8D9C-4A3D-8BAE-9627E818F767}" name="AG Ref No." dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{C458FCAF-DCE1-469B-AD89-03ED0B941816}" name="Age" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7384EF93-7717-4C50-89EF-BCFA6A3B1B22}" name="Year(s)" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6F4A5391-C5C3-4A11-A760-B582C4B8722F}" name="Men" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{2CC1F6E2-14F1-421F-8DD7-62E44379A787}" name="Women" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8B3DAEFC-581B-402C-B6D8-3BE90D16832D}" name="Table2" displayName="Table2" ref="A4:D12" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A4:D12" xr:uid="{4BD89E54-741A-4CE7-81E6-93DE189F141F}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{76A2C90A-5BCF-46D4-9899-B92DA2F11CDC}" name="YEAR" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{C481D22B-608A-475C-BFB8-F74F23863CAC}" name="FIELD SIZE" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{F68FBDA7-2593-48A4-9CE7-0B1FCAC3DD97}" name="&quot;CUT-OFF TIME&quot;*" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{D7CAE966-1EC3-4BA6-90FF-E9C0B5BB871F}" name="QUALIFIERS NOT ACCEPTED" dataDxfId="31"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{42ED1202-1471-4032-B954-14568DD03C17}" name="Table3" displayName="Table3" ref="A4:C15" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
-  <autoFilter ref="A4:C15" xr:uid="{7B5350B7-A0FC-433D-A5F0-FE41276BFEDF}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3FFEE83F-EA83-48EE-9835-8E7C41684F00}" name="Age Group" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{A4CDB995-4791-49EB-8F20-0F0272AB9FB1}" name="MEN" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{4617F89F-6262-440B-8BB3-CBAD5A2AA9E6}" name="WOMEN" dataDxfId="26"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FF7DBF91-7FDC-4BEA-B0D3-952E1FD3B3A6}" name="Table4" displayName="Table4" ref="I4:K15" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="I4:K15" xr:uid="{F6BB4E07-146D-4746-8CC4-E05E3F16557F}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E7DE7640-B9C2-495F-82B4-6263CCF819BF}" name="Age Group" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{28FC9761-D671-4390-83F1-654565E76239}" name="MEN" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{A5A0BCCF-E68B-4FE7-83CC-AE297FB16E2E}" name="WOMEN" dataDxfId="21"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{842E0509-0DAB-40B3-8B32-0689BF5A5CFF}" name="Table5" displayName="Table5" ref="Q4:S15" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="Q4:S15" xr:uid="{81A9722F-45A3-433B-9C69-98AEF52383AC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FCBC2632-97C5-440D-9574-DCC5C9476E1C}" name="AGE GROUP" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{5EC137FE-185A-4EA1-AA5C-813F10DBFC18}" name="MEN" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{1ADF95C7-3BEC-40D0-B246-6032AD2C604B}" name="WOMEN" dataDxfId="16"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{05AC6517-A111-4017-B412-51FDF10A2405}" name="Table6" displayName="Table6" ref="E4:G87" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="E4:G87" xr:uid="{D31C94E5-7D81-415B-8D1D-039D4EF66E19}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F314AFF1-1A97-46F3-909B-13048F24B7B7}" name="Age" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{AF01B4CB-98C8-4A3C-943A-9B61B79BC73A}" name="Men" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{851E6146-F745-4907-B6EE-A3B841FE653A}" name="Women" dataDxfId="11"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{039B3C15-8BE3-4FDA-8D77-2667238F62D6}" name="Table7" displayName="Table7" ref="M4:O87" totalsRowShown="0">
-  <autoFilter ref="M4:O87" xr:uid="{4EEF452D-9B92-427D-89B5-BEF3706CC6AC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{2B1729D4-FABD-4743-8F9B-A114A5F20149}" name="Age"/>
-    <tableColumn id="2" xr3:uid="{E114616D-74B2-400C-8116-BE1353E1E7BF}" name="Men"/>
-    <tableColumn id="3" xr3:uid="{8147C7CD-4226-478A-BB28-587AD04BFADD}" name="Women"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7E940803-55B0-4DE3-9F18-7FDF262391E6}" name="Table8" displayName="Table8" ref="U4:W87" totalsRowShown="0">
   <autoFilter ref="U4:W87" xr:uid="{61C26B11-D61B-430C-9B89-0BDB1B81FE6F}"/>
   <tableColumns count="3">
@@ -21209,7 +21827,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BC5882D9-7DB3-4E78-A9A9-8457EB714AB3}" name="Table810" displayName="Table810" ref="Y4:AE87" totalsRowShown="0">
   <autoFilter ref="Y4:AE87" xr:uid="{DDD8E665-4B76-4E21-9A1B-036A5785F7F8}"/>
   <tableColumns count="7">
@@ -21220,12 +21838,171 @@
     <tableColumn id="3" xr3:uid="{703A4925-2699-4887-9D2B-768209D06CDC}" name="Women 2003 -2012">
       <calculatedColumnFormula>Table6[[#This Row],[Women]]+$S$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{A02A78FF-921F-4560-97F5-35AC8CC93734}" name="Men 2013-2019" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{05E3904F-AD7E-43E2-AB64-B1DA7FE28076}" name="Women 2013-2019" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{F56990F5-3BB6-440B-9FD1-F1853F7863AB}" name="Women 2013-2020" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{DCE68EF4-083E-4DA0-8D1A-0A3C56A41D22}" name="Women 2013-2021" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A02A78FF-921F-4560-97F5-35AC8CC93734}" name="Men 2013-2019" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{05E3904F-AD7E-43E2-AB64-B1DA7FE28076}" name="Women 2013-2019" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{F56990F5-3BB6-440B-9FD1-F1853F7863AB}" name="Women 2013-2020" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{DCE68EF4-083E-4DA0-8D1A-0A3C56A41D22}" name="Women 2013-2021" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{945CDC40-C170-4D74-BF4F-2A501FDC2EE5}" name="Table81011" displayName="Table81011" ref="AG4:AJ253" totalsRowShown="0">
+  <autoFilter ref="AG4:AJ253" xr:uid="{0D6CC08B-E199-4CA5-92C7-B34C714671A0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B3D04435-650B-45FD-A98E-E0EC10C3547E}" name="Age"/>
+    <tableColumn id="6" xr3:uid="{18C002B2-A54A-4967-B8BC-024E0ED82E13}" name="Year" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{AA207F6A-07E3-4A95-B636-24C8CCC8B945}" name="Men">
+      <calculatedColumnFormula>Table6[[#This Row],[Men]]+$S$1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{9B32EE09-A5B9-4DC3-95D8-2349E4A40D6E}" name="Women">
+      <calculatedColumnFormula>Table6[[#This Row],[Women]]+$S$1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C47162FF-5668-4B36-A460-2609D44826EC}" name="Table11" displayName="Table11" ref="A1:E250" totalsRowShown="0" dataDxfId="17">
+  <autoFilter ref="A1:E250" xr:uid="{512EA7CA-480E-423A-92C9-18C2E1562366}"/>
+  <tableColumns count="5">
+    <tableColumn id="5" xr3:uid="{312D51B1-8D9C-4A3D-8BAE-9627E818F767}" name="AG Ref No." dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{C458FCAF-DCE1-469B-AD89-03ED0B941816}" name="Age" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7384EF93-7717-4C50-89EF-BCFA6A3B1B22}" name="Year(s)" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{6F4A5391-C5C3-4A11-A760-B582C4B8722F}" name="Men" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{2CC1F6E2-14F1-421F-8DD7-62E44379A787}" name="Women" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{86C14095-1EAE-4E61-9F65-E04ABBC0B9CD}" name="Table413" displayName="Table413" ref="E2:F13" totalsRowShown="0">
+  <autoFilter ref="E2:F13" xr:uid="{8DCFB31A-B430-423E-82DC-9A790220481D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2833AC45-5A06-42FD-A6C0-7F5DF83F1992}" name="AG Ref No."/>
+    <tableColumn id="2" xr3:uid="{5C97F61D-4E67-4C86-8E4A-900E7F20EE7D}" name="Age Group"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{A9ED582E-18BF-432B-9D8A-0231BE28CFE1}" name="Table514" displayName="Table514" ref="A2:C85" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A2:C85" xr:uid="{B0C3BA94-6F86-4DE0-914F-97C889DD565F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A33E98C7-44FA-42F8-887F-28788AA494BB}" name="AG Ref No." dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E17837E2-BB0B-41EB-8A40-DAEBE224E276}" name="Age" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9D0FFBFF-35E4-4773-A154-4C4B004F6271}" name="Age Group" dataDxfId="6">
+      <calculatedColumnFormula>VLOOKUP(Bos_Age_Groups!$A3,Table413[],2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B84E7CC6-AA43-4E20-9F1B-E793456AE462}" name="Table516" displayName="Table516" ref="A2:C85" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A2:C85" xr:uid="{B0C3BA94-6F86-4DE0-914F-97C889DD565F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{36E71FD6-36BB-4BFF-9329-3CBB14042F87}" name="AG Ref No." dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3841C53D-2A71-4283-8CA3-EBD3F1592253}" name="Age" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{AC0A4146-EFF7-42DA-B338-46ADB4BE3A37}" name="Age Group" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP([1]Bos_Age_Groups!$A3,Table415[],2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F0BBD01-FBED-4417-A64E-216A3B1D2B76}" name="Table1" displayName="Table1" ref="A4:G53" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+  <autoFilter ref="A4:G53" xr:uid="{3F6DDC19-D566-4BC4-965F-870509961C56}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{BCD665A8-DC48-4371-BEC9-85E36B63290A}" name="YEAR" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{06798F71-F324-43C3-8BA2-6CE198AE158F}" name="TOTAL ENTRANTS" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{2296CF0F-522F-4A8B-B331-2AA39E601128}" name="TOTAL ENTRANTS: MEN" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{5F300890-7957-4BA9-9943-73007F1A1C4F}" name="TOTAL ENTRANTS: WOMEN" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{92948D5C-4BB1-43D5-A11D-C418A80F5517}" name="TOTAL FINISHERS" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{BAF4C57E-65CB-47A9-A209-66F6AC1AAF88}" name="TOTAL FINISHERS: MEN" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{59C23AF6-67B2-4BC8-A5FD-176ED3F381F6}" name="TOTAL FINISHERS: WOMEN" dataDxfId="49"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8B3DAEFC-581B-402C-B6D8-3BE90D16832D}" name="Table2" displayName="Table2" ref="A4:D12" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A4:D12" xr:uid="{4BD89E54-741A-4CE7-81E6-93DE189F141F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{76A2C90A-5BCF-46D4-9899-B92DA2F11CDC}" name="YEAR" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{C481D22B-608A-475C-BFB8-F74F23863CAC}" name="FIELD SIZE" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{F68FBDA7-2593-48A4-9CE7-0B1FCAC3DD97}" name="&quot;CUT-OFF TIME&quot;*" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{D7CAE966-1EC3-4BA6-90FF-E9C0B5BB871F}" name="QUALIFIERS NOT ACCEPTED" dataDxfId="43"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{42ED1202-1471-4032-B954-14568DD03C17}" name="Table3" displayName="Table3" ref="A4:C15" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A4:C15" xr:uid="{7B5350B7-A0FC-433D-A5F0-FE41276BFEDF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3FFEE83F-EA83-48EE-9835-8E7C41684F00}" name="Age Group" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{A4CDB995-4791-49EB-8F20-0F0272AB9FB1}" name="MEN" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{4617F89F-6262-440B-8BB3-CBAD5A2AA9E6}" name="WOMEN" dataDxfId="38"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{FF7DBF91-7FDC-4BEA-B0D3-952E1FD3B3A6}" name="Table4" displayName="Table4" ref="I4:K15" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="I4:K15" xr:uid="{F6BB4E07-146D-4746-8CC4-E05E3F16557F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E7DE7640-B9C2-495F-82B4-6263CCF819BF}" name="Age Group" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{28FC9761-D671-4390-83F1-654565E76239}" name="MEN" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{A5A0BCCF-E68B-4FE7-83CC-AE297FB16E2E}" name="WOMEN" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{842E0509-0DAB-40B3-8B32-0689BF5A5CFF}" name="Table5" displayName="Table5" ref="Q4:S15" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="Q4:S15" xr:uid="{81A9722F-45A3-433B-9C69-98AEF52383AC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FCBC2632-97C5-440D-9574-DCC5C9476E1C}" name="AGE GROUP" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{5EC137FE-185A-4EA1-AA5C-813F10DBFC18}" name="MEN" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{1ADF95C7-3BEC-40D0-B246-6032AD2C604B}" name="WOMEN" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{05AC6517-A111-4017-B412-51FDF10A2405}" name="Table6" displayName="Table6" ref="E4:G87" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="E4:G87" xr:uid="{D31C94E5-7D81-415B-8D1D-039D4EF66E19}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F314AFF1-1A97-46F3-909B-13048F24B7B7}" name="Age" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{AF01B4CB-98C8-4A3C-943A-9B61B79BC73A}" name="Men" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{851E6146-F745-4907-B6EE-A3B841FE653A}" name="Women" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{039B3C15-8BE3-4FDA-8D77-2667238F62D6}" name="Table7" displayName="Table7" ref="M4:O87" totalsRowShown="0">
+  <autoFilter ref="M4:O87" xr:uid="{4EEF452D-9B92-427D-89B5-BEF3706CC6AC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2B1729D4-FABD-4743-8F9B-A114A5F20149}" name="Age"/>
+    <tableColumn id="2" xr3:uid="{E114616D-74B2-400C-8116-BE1353E1E7BF}" name="Men"/>
+    <tableColumn id="3" xr3:uid="{8147C7CD-4226-478A-BB28-587AD04BFADD}" name="Women"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -21525,6 +22302,1115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FEB2AC-E6E8-4A9B-9DCC-4280359C0C17}">
+  <dimension ref="A1:F85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.3671875" customWidth="1"/>
+    <col min="3" max="3" width="11.15625" customWidth="1"/>
+    <col min="5" max="5" width="11.05078125" customWidth="1"/>
+    <col min="6" max="6" width="10.83984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="40">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40">
+        <v>18</v>
+      </c>
+      <c r="C3" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A3,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="40">
+        <v>1</v>
+      </c>
+      <c r="B4" s="40">
+        <v>19</v>
+      </c>
+      <c r="C4" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A4,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="40">
+        <v>1</v>
+      </c>
+      <c r="B5" s="40">
+        <v>20</v>
+      </c>
+      <c r="C5" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A5,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="40">
+        <v>1</v>
+      </c>
+      <c r="B6" s="40">
+        <v>21</v>
+      </c>
+      <c r="C6" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A6,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="40">
+        <v>1</v>
+      </c>
+      <c r="B7" s="40">
+        <v>22</v>
+      </c>
+      <c r="C7" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A7,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="40">
+        <v>1</v>
+      </c>
+      <c r="B8" s="40">
+        <v>23</v>
+      </c>
+      <c r="C8" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A8,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="40">
+        <v>1</v>
+      </c>
+      <c r="B9" s="40">
+        <v>24</v>
+      </c>
+      <c r="C9" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A9,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="40">
+        <v>1</v>
+      </c>
+      <c r="B10" s="40">
+        <v>25</v>
+      </c>
+      <c r="C10" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A10,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="40">
+        <v>26</v>
+      </c>
+      <c r="C11" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A11,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="40">
+        <v>1</v>
+      </c>
+      <c r="B12" s="40">
+        <v>27</v>
+      </c>
+      <c r="C12" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A12,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="40">
+        <v>1</v>
+      </c>
+      <c r="B13" s="40">
+        <v>28</v>
+      </c>
+      <c r="C13" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A13,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="40">
+        <v>1</v>
+      </c>
+      <c r="B14" s="40">
+        <v>29</v>
+      </c>
+      <c r="C14" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A14,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="40">
+        <v>1</v>
+      </c>
+      <c r="B15" s="40">
+        <v>30</v>
+      </c>
+      <c r="C15" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A15,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="40">
+        <v>1</v>
+      </c>
+      <c r="B16" s="40">
+        <v>31</v>
+      </c>
+      <c r="C16" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A16,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="40">
+        <v>1</v>
+      </c>
+      <c r="B17" s="40">
+        <v>32</v>
+      </c>
+      <c r="C17" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A17,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="40">
+        <v>1</v>
+      </c>
+      <c r="B18" s="40">
+        <v>33</v>
+      </c>
+      <c r="C18" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A18,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="40">
+        <v>1</v>
+      </c>
+      <c r="B19" s="40">
+        <v>34</v>
+      </c>
+      <c r="C19" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A19,Table415[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="40">
+        <v>2</v>
+      </c>
+      <c r="B20" s="40">
+        <v>35</v>
+      </c>
+      <c r="C20" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A20,Table415[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="40">
+        <v>2</v>
+      </c>
+      <c r="B21" s="40">
+        <v>36</v>
+      </c>
+      <c r="C21" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A21,Table415[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="40">
+        <v>2</v>
+      </c>
+      <c r="B22" s="40">
+        <v>37</v>
+      </c>
+      <c r="C22" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A22,Table415[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="40">
+        <v>2</v>
+      </c>
+      <c r="B23" s="40">
+        <v>38</v>
+      </c>
+      <c r="C23" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A23,Table415[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="40">
+        <v>2</v>
+      </c>
+      <c r="B24" s="40">
+        <v>39</v>
+      </c>
+      <c r="C24" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A24,Table415[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="40">
+        <v>3</v>
+      </c>
+      <c r="B25" s="40">
+        <v>40</v>
+      </c>
+      <c r="C25" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A25,Table415[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="40">
+        <v>3</v>
+      </c>
+      <c r="B26" s="40">
+        <v>41</v>
+      </c>
+      <c r="C26" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A26,Table415[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="40">
+        <v>3</v>
+      </c>
+      <c r="B27" s="40">
+        <v>42</v>
+      </c>
+      <c r="C27" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A27,Table415[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="40">
+        <v>3</v>
+      </c>
+      <c r="B28" s="40">
+        <v>43</v>
+      </c>
+      <c r="C28" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A28,Table415[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="40">
+        <v>3</v>
+      </c>
+      <c r="B29" s="40">
+        <v>44</v>
+      </c>
+      <c r="C29" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A29,Table415[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="40">
+        <v>4</v>
+      </c>
+      <c r="B30" s="40">
+        <v>45</v>
+      </c>
+      <c r="C30" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A30,Table415[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="40">
+        <v>4</v>
+      </c>
+      <c r="B31" s="40">
+        <v>46</v>
+      </c>
+      <c r="C31" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A31,Table415[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="40">
+        <v>4</v>
+      </c>
+      <c r="B32" s="40">
+        <v>47</v>
+      </c>
+      <c r="C32" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A32,Table415[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="40">
+        <v>4</v>
+      </c>
+      <c r="B33" s="40">
+        <v>48</v>
+      </c>
+      <c r="C33" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A33,Table415[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="40">
+        <v>4</v>
+      </c>
+      <c r="B34" s="40">
+        <v>49</v>
+      </c>
+      <c r="C34" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A34,Table415[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="40">
+        <v>5</v>
+      </c>
+      <c r="B35" s="40">
+        <v>50</v>
+      </c>
+      <c r="C35" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A35,Table415[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="40">
+        <v>5</v>
+      </c>
+      <c r="B36" s="40">
+        <v>51</v>
+      </c>
+      <c r="C36" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A36,Table415[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="40">
+        <v>5</v>
+      </c>
+      <c r="B37" s="40">
+        <v>52</v>
+      </c>
+      <c r="C37" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A37,Table415[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="40">
+        <v>5</v>
+      </c>
+      <c r="B38" s="40">
+        <v>53</v>
+      </c>
+      <c r="C38" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A38,Table415[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="40">
+        <v>5</v>
+      </c>
+      <c r="B39" s="40">
+        <v>54</v>
+      </c>
+      <c r="C39" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A39,Table415[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="40">
+        <v>6</v>
+      </c>
+      <c r="B40" s="40">
+        <v>55</v>
+      </c>
+      <c r="C40" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A40,Table415[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="40">
+        <v>6</v>
+      </c>
+      <c r="B41" s="40">
+        <v>56</v>
+      </c>
+      <c r="C41" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A41,Table415[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="40">
+        <v>6</v>
+      </c>
+      <c r="B42" s="40">
+        <v>57</v>
+      </c>
+      <c r="C42" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A42,Table415[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="40">
+        <v>6</v>
+      </c>
+      <c r="B43" s="40">
+        <v>58</v>
+      </c>
+      <c r="C43" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A43,Table415[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="40">
+        <v>6</v>
+      </c>
+      <c r="B44" s="40">
+        <v>59</v>
+      </c>
+      <c r="C44" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A44,Table415[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="40">
+        <v>7</v>
+      </c>
+      <c r="B45" s="40">
+        <v>60</v>
+      </c>
+      <c r="C45" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A45,Table415[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="40">
+        <v>7</v>
+      </c>
+      <c r="B46" s="40">
+        <v>61</v>
+      </c>
+      <c r="C46" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A46,Table415[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="40">
+        <v>7</v>
+      </c>
+      <c r="B47" s="40">
+        <v>62</v>
+      </c>
+      <c r="C47" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A47,Table415[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="40">
+        <v>7</v>
+      </c>
+      <c r="B48" s="40">
+        <v>63</v>
+      </c>
+      <c r="C48" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A48,Table415[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="40">
+        <v>7</v>
+      </c>
+      <c r="B49" s="40">
+        <v>64</v>
+      </c>
+      <c r="C49" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A49,Table415[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="40">
+        <v>8</v>
+      </c>
+      <c r="B50" s="40">
+        <v>65</v>
+      </c>
+      <c r="C50" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A50,Table415[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="40">
+        <v>8</v>
+      </c>
+      <c r="B51" s="40">
+        <v>66</v>
+      </c>
+      <c r="C51" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A51,Table415[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="40">
+        <v>8</v>
+      </c>
+      <c r="B52" s="40">
+        <v>67</v>
+      </c>
+      <c r="C52" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A52,Table415[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="40">
+        <v>8</v>
+      </c>
+      <c r="B53" s="40">
+        <v>68</v>
+      </c>
+      <c r="C53" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A53,Table415[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="40">
+        <v>8</v>
+      </c>
+      <c r="B54" s="40">
+        <v>69</v>
+      </c>
+      <c r="C54" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A54,Table415[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="40">
+        <v>9</v>
+      </c>
+      <c r="B55" s="40">
+        <v>70</v>
+      </c>
+      <c r="C55" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A55,Table415[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="40">
+        <v>9</v>
+      </c>
+      <c r="B56" s="40">
+        <v>71</v>
+      </c>
+      <c r="C56" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A56,Table415[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="40">
+        <v>9</v>
+      </c>
+      <c r="B57" s="40">
+        <v>72</v>
+      </c>
+      <c r="C57" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A57,Table415[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="40">
+        <v>9</v>
+      </c>
+      <c r="B58" s="40">
+        <v>73</v>
+      </c>
+      <c r="C58" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A58,Table415[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="40">
+        <v>9</v>
+      </c>
+      <c r="B59" s="40">
+        <v>74</v>
+      </c>
+      <c r="C59" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A59,Table415[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="40">
+        <v>10</v>
+      </c>
+      <c r="B60" s="40">
+        <v>75</v>
+      </c>
+      <c r="C60" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A60,Table415[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="40">
+        <v>10</v>
+      </c>
+      <c r="B61" s="40">
+        <v>76</v>
+      </c>
+      <c r="C61" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A61,Table415[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="40">
+        <v>10</v>
+      </c>
+      <c r="B62" s="40">
+        <v>77</v>
+      </c>
+      <c r="C62" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A62,Table415[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="40">
+        <v>10</v>
+      </c>
+      <c r="B63" s="40">
+        <v>78</v>
+      </c>
+      <c r="C63" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A63,Table415[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="40">
+        <v>10</v>
+      </c>
+      <c r="B64" s="40">
+        <v>79</v>
+      </c>
+      <c r="C64" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A64,Table415[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="40">
+        <v>11</v>
+      </c>
+      <c r="B65" s="40">
+        <v>80</v>
+      </c>
+      <c r="C65" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A65,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="40">
+        <v>11</v>
+      </c>
+      <c r="B66" s="40">
+        <v>81</v>
+      </c>
+      <c r="C66" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A66,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="40">
+        <v>11</v>
+      </c>
+      <c r="B67" s="40">
+        <v>82</v>
+      </c>
+      <c r="C67" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A67,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="40">
+        <v>11</v>
+      </c>
+      <c r="B68" s="40">
+        <v>83</v>
+      </c>
+      <c r="C68" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A68,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="40">
+        <v>11</v>
+      </c>
+      <c r="B69" s="40">
+        <v>84</v>
+      </c>
+      <c r="C69" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A69,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="40">
+        <v>11</v>
+      </c>
+      <c r="B70" s="40">
+        <v>85</v>
+      </c>
+      <c r="C70" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A70,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="40">
+        <v>11</v>
+      </c>
+      <c r="B71" s="40">
+        <v>86</v>
+      </c>
+      <c r="C71" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A71,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="40">
+        <v>11</v>
+      </c>
+      <c r="B72" s="40">
+        <v>87</v>
+      </c>
+      <c r="C72" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A72,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="40">
+        <v>11</v>
+      </c>
+      <c r="B73" s="40">
+        <v>88</v>
+      </c>
+      <c r="C73" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A73,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="40">
+        <v>11</v>
+      </c>
+      <c r="B74" s="40">
+        <v>89</v>
+      </c>
+      <c r="C74" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A74,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="40">
+        <v>11</v>
+      </c>
+      <c r="B75" s="40">
+        <v>90</v>
+      </c>
+      <c r="C75" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A75,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="40">
+        <v>11</v>
+      </c>
+      <c r="B76" s="40">
+        <v>91</v>
+      </c>
+      <c r="C76" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A76,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="40">
+        <v>11</v>
+      </c>
+      <c r="B77" s="40">
+        <v>92</v>
+      </c>
+      <c r="C77" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A77,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="40">
+        <v>11</v>
+      </c>
+      <c r="B78" s="40">
+        <v>93</v>
+      </c>
+      <c r="C78" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A78,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="40">
+        <v>11</v>
+      </c>
+      <c r="B79" s="40">
+        <v>94</v>
+      </c>
+      <c r="C79" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A79,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="40">
+        <v>11</v>
+      </c>
+      <c r="B80" s="40">
+        <v>95</v>
+      </c>
+      <c r="C80" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A80,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="40">
+        <v>11</v>
+      </c>
+      <c r="B81" s="40">
+        <v>96</v>
+      </c>
+      <c r="C81" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A81,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="40">
+        <v>11</v>
+      </c>
+      <c r="B82" s="40">
+        <v>97</v>
+      </c>
+      <c r="C82" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A82,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="40">
+        <v>11</v>
+      </c>
+      <c r="B83" s="40">
+        <v>98</v>
+      </c>
+      <c r="C83" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A83,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="40">
+        <v>11</v>
+      </c>
+      <c r="B84" s="40">
+        <v>99</v>
+      </c>
+      <c r="C84" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A84,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="40">
+        <v>11</v>
+      </c>
+      <c r="B85" s="40">
+        <v>100</v>
+      </c>
+      <c r="C85" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A85,Table415[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D3F986-CCCF-4C01-8BD2-A6865EC131A0}">
   <dimension ref="A1:G55"/>
   <sheetViews>
@@ -22732,7 +24618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E524554B-0D67-44C3-8A8F-24AE346C46CC}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -22892,7 +24778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B43F26-FCFD-4241-9BAA-22AFC86074B0}">
   <dimension ref="A1:AJ253"/>
   <sheetViews>
@@ -22945,21 +24831,21 @@
       </c>
     </row>
     <row r="3" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="34">
+      <c r="A3" s="35">
         <v>2020</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="I3" s="35" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="I3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="Q3" s="36" t="s">
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="Q3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="18" t="s">
@@ -31380,12 +33266,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F81623-E2C1-4309-B7AD-043E596483C3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{567399F0-F739-416E-81B4-FF71CE98CD92}">
   <dimension ref="A1:E250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -34243,7 +36141,7 @@
       <c r="B168" s="32">
         <v>18</v>
       </c>
-      <c r="C168" s="37" t="s">
+      <c r="C168" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D168" s="33">
@@ -34260,7 +36158,7 @@
       <c r="B169" s="32">
         <v>19</v>
       </c>
-      <c r="C169" s="37" t="s">
+      <c r="C169" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D169" s="33">
@@ -34277,7 +36175,7 @@
       <c r="B170" s="32">
         <v>20</v>
       </c>
-      <c r="C170" s="37" t="s">
+      <c r="C170" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D170" s="33">
@@ -34294,7 +36192,7 @@
       <c r="B171" s="32">
         <v>21</v>
       </c>
-      <c r="C171" s="37" t="s">
+      <c r="C171" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D171" s="33">
@@ -34311,7 +36209,7 @@
       <c r="B172" s="32">
         <v>22</v>
       </c>
-      <c r="C172" s="37" t="s">
+      <c r="C172" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D172" s="33">
@@ -34328,7 +36226,7 @@
       <c r="B173" s="32">
         <v>23</v>
       </c>
-      <c r="C173" s="37" t="s">
+      <c r="C173" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D173" s="33">
@@ -34345,7 +36243,7 @@
       <c r="B174" s="32">
         <v>24</v>
       </c>
-      <c r="C174" s="37" t="s">
+      <c r="C174" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D174" s="33">
@@ -34362,7 +36260,7 @@
       <c r="B175" s="32">
         <v>25</v>
       </c>
-      <c r="C175" s="37" t="s">
+      <c r="C175" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D175" s="33">
@@ -34379,7 +36277,7 @@
       <c r="B176" s="32">
         <v>26</v>
       </c>
-      <c r="C176" s="37" t="s">
+      <c r="C176" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D176" s="33">
@@ -34396,7 +36294,7 @@
       <c r="B177" s="32">
         <v>27</v>
       </c>
-      <c r="C177" s="37" t="s">
+      <c r="C177" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D177" s="33">
@@ -34413,7 +36311,7 @@
       <c r="B178" s="32">
         <v>28</v>
       </c>
-      <c r="C178" s="37" t="s">
+      <c r="C178" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D178" s="33">
@@ -34430,7 +36328,7 @@
       <c r="B179" s="32">
         <v>29</v>
       </c>
-      <c r="C179" s="37" t="s">
+      <c r="C179" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D179" s="33">
@@ -34447,7 +36345,7 @@
       <c r="B180" s="32">
         <v>30</v>
       </c>
-      <c r="C180" s="37" t="s">
+      <c r="C180" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D180" s="33">
@@ -34464,7 +36362,7 @@
       <c r="B181" s="32">
         <v>31</v>
       </c>
-      <c r="C181" s="37" t="s">
+      <c r="C181" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D181" s="33">
@@ -34481,7 +36379,7 @@
       <c r="B182" s="32">
         <v>32</v>
       </c>
-      <c r="C182" s="37" t="s">
+      <c r="C182" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D182" s="33">
@@ -34498,7 +36396,7 @@
       <c r="B183" s="32">
         <v>33</v>
       </c>
-      <c r="C183" s="37" t="s">
+      <c r="C183" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D183" s="33">
@@ -34515,7 +36413,7 @@
       <c r="B184" s="32">
         <v>34</v>
       </c>
-      <c r="C184" s="37" t="s">
+      <c r="C184" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D184" s="33">
@@ -34532,7 +36430,7 @@
       <c r="B185" s="32">
         <v>35</v>
       </c>
-      <c r="C185" s="37" t="s">
+      <c r="C185" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D185" s="33">
@@ -34549,7 +36447,7 @@
       <c r="B186" s="32">
         <v>36</v>
       </c>
-      <c r="C186" s="37" t="s">
+      <c r="C186" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D186" s="33">
@@ -34566,7 +36464,7 @@
       <c r="B187" s="32">
         <v>37</v>
       </c>
-      <c r="C187" s="37" t="s">
+      <c r="C187" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D187" s="33">
@@ -34583,7 +36481,7 @@
       <c r="B188" s="32">
         <v>38</v>
       </c>
-      <c r="C188" s="37" t="s">
+      <c r="C188" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D188" s="33">
@@ -34600,7 +36498,7 @@
       <c r="B189" s="32">
         <v>39</v>
       </c>
-      <c r="C189" s="37" t="s">
+      <c r="C189" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D189" s="33">
@@ -34617,7 +36515,7 @@
       <c r="B190" s="32">
         <v>40</v>
       </c>
-      <c r="C190" s="37" t="s">
+      <c r="C190" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D190" s="33">
@@ -34634,7 +36532,7 @@
       <c r="B191" s="32">
         <v>41</v>
       </c>
-      <c r="C191" s="37" t="s">
+      <c r="C191" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D191" s="33">
@@ -34651,7 +36549,7 @@
       <c r="B192" s="32">
         <v>42</v>
       </c>
-      <c r="C192" s="37" t="s">
+      <c r="C192" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D192" s="33">
@@ -34668,7 +36566,7 @@
       <c r="B193" s="32">
         <v>43</v>
       </c>
-      <c r="C193" s="37" t="s">
+      <c r="C193" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D193" s="33">
@@ -34685,7 +36583,7 @@
       <c r="B194" s="32">
         <v>44</v>
       </c>
-      <c r="C194" s="37" t="s">
+      <c r="C194" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D194" s="33">
@@ -34702,7 +36600,7 @@
       <c r="B195" s="32">
         <v>45</v>
       </c>
-      <c r="C195" s="37" t="s">
+      <c r="C195" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D195" s="33">
@@ -34719,7 +36617,7 @@
       <c r="B196" s="32">
         <v>46</v>
       </c>
-      <c r="C196" s="37" t="s">
+      <c r="C196" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D196" s="33">
@@ -34736,7 +36634,7 @@
       <c r="B197" s="32">
         <v>47</v>
       </c>
-      <c r="C197" s="37" t="s">
+      <c r="C197" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D197" s="33">
@@ -34753,7 +36651,7 @@
       <c r="B198" s="32">
         <v>48</v>
       </c>
-      <c r="C198" s="37" t="s">
+      <c r="C198" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D198" s="33">
@@ -34770,7 +36668,7 @@
       <c r="B199" s="32">
         <v>49</v>
       </c>
-      <c r="C199" s="37" t="s">
+      <c r="C199" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D199" s="33">
@@ -34787,7 +36685,7 @@
       <c r="B200" s="32">
         <v>50</v>
       </c>
-      <c r="C200" s="37" t="s">
+      <c r="C200" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D200" s="33">
@@ -34804,7 +36702,7 @@
       <c r="B201" s="32">
         <v>51</v>
       </c>
-      <c r="C201" s="37" t="s">
+      <c r="C201" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D201" s="33">
@@ -34821,7 +36719,7 @@
       <c r="B202" s="32">
         <v>52</v>
       </c>
-      <c r="C202" s="37" t="s">
+      <c r="C202" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D202" s="33">
@@ -34838,7 +36736,7 @@
       <c r="B203" s="32">
         <v>53</v>
       </c>
-      <c r="C203" s="37" t="s">
+      <c r="C203" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D203" s="33">
@@ -34855,7 +36753,7 @@
       <c r="B204" s="32">
         <v>54</v>
       </c>
-      <c r="C204" s="37" t="s">
+      <c r="C204" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D204" s="33">
@@ -34872,7 +36770,7 @@
       <c r="B205" s="32">
         <v>55</v>
       </c>
-      <c r="C205" s="37" t="s">
+      <c r="C205" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D205" s="33">
@@ -34889,7 +36787,7 @@
       <c r="B206" s="32">
         <v>56</v>
       </c>
-      <c r="C206" s="37" t="s">
+      <c r="C206" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D206" s="33">
@@ -34906,7 +36804,7 @@
       <c r="B207" s="32">
         <v>57</v>
       </c>
-      <c r="C207" s="37" t="s">
+      <c r="C207" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D207" s="33">
@@ -34923,7 +36821,7 @@
       <c r="B208" s="32">
         <v>58</v>
       </c>
-      <c r="C208" s="37" t="s">
+      <c r="C208" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D208" s="33">
@@ -34940,7 +36838,7 @@
       <c r="B209" s="32">
         <v>59</v>
       </c>
-      <c r="C209" s="37" t="s">
+      <c r="C209" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D209" s="33">
@@ -34957,7 +36855,7 @@
       <c r="B210" s="32">
         <v>60</v>
       </c>
-      <c r="C210" s="37" t="s">
+      <c r="C210" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D210" s="33">
@@ -34974,7 +36872,7 @@
       <c r="B211" s="32">
         <v>61</v>
       </c>
-      <c r="C211" s="37" t="s">
+      <c r="C211" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D211" s="33">
@@ -34991,7 +36889,7 @@
       <c r="B212" s="32">
         <v>62</v>
       </c>
-      <c r="C212" s="37" t="s">
+      <c r="C212" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D212" s="33">
@@ -35008,7 +36906,7 @@
       <c r="B213" s="32">
         <v>63</v>
       </c>
-      <c r="C213" s="37" t="s">
+      <c r="C213" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D213" s="33">
@@ -35025,7 +36923,7 @@
       <c r="B214" s="32">
         <v>64</v>
       </c>
-      <c r="C214" s="37" t="s">
+      <c r="C214" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D214" s="33">
@@ -35042,7 +36940,7 @@
       <c r="B215" s="32">
         <v>65</v>
       </c>
-      <c r="C215" s="37" t="s">
+      <c r="C215" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D215" s="33">
@@ -35059,7 +36957,7 @@
       <c r="B216" s="32">
         <v>66</v>
       </c>
-      <c r="C216" s="37" t="s">
+      <c r="C216" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D216" s="33">
@@ -35076,7 +36974,7 @@
       <c r="B217" s="32">
         <v>67</v>
       </c>
-      <c r="C217" s="37" t="s">
+      <c r="C217" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D217" s="33">
@@ -35093,7 +36991,7 @@
       <c r="B218" s="32">
         <v>68</v>
       </c>
-      <c r="C218" s="37" t="s">
+      <c r="C218" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D218" s="33">
@@ -35110,7 +37008,7 @@
       <c r="B219" s="32">
         <v>69</v>
       </c>
-      <c r="C219" s="37" t="s">
+      <c r="C219" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D219" s="33">
@@ -35127,7 +37025,7 @@
       <c r="B220" s="32">
         <v>70</v>
       </c>
-      <c r="C220" s="37" t="s">
+      <c r="C220" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D220" s="33">
@@ -35144,7 +37042,7 @@
       <c r="B221" s="32">
         <v>71</v>
       </c>
-      <c r="C221" s="37" t="s">
+      <c r="C221" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D221" s="33">
@@ -35161,7 +37059,7 @@
       <c r="B222" s="32">
         <v>72</v>
       </c>
-      <c r="C222" s="37" t="s">
+      <c r="C222" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D222" s="33">
@@ -35178,7 +37076,7 @@
       <c r="B223" s="32">
         <v>73</v>
       </c>
-      <c r="C223" s="37" t="s">
+      <c r="C223" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D223" s="33">
@@ -35195,7 +37093,7 @@
       <c r="B224" s="32">
         <v>74</v>
       </c>
-      <c r="C224" s="37" t="s">
+      <c r="C224" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D224" s="33">
@@ -35212,7 +37110,7 @@
       <c r="B225" s="32">
         <v>75</v>
       </c>
-      <c r="C225" s="37" t="s">
+      <c r="C225" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D225" s="33">
@@ -35229,7 +37127,7 @@
       <c r="B226" s="32">
         <v>76</v>
       </c>
-      <c r="C226" s="37" t="s">
+      <c r="C226" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D226" s="33">
@@ -35246,7 +37144,7 @@
       <c r="B227" s="32">
         <v>77</v>
       </c>
-      <c r="C227" s="37" t="s">
+      <c r="C227" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D227" s="33">
@@ -35263,7 +37161,7 @@
       <c r="B228" s="32">
         <v>78</v>
       </c>
-      <c r="C228" s="37" t="s">
+      <c r="C228" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D228" s="33">
@@ -35280,7 +37178,7 @@
       <c r="B229" s="32">
         <v>79</v>
       </c>
-      <c r="C229" s="37" t="s">
+      <c r="C229" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D229" s="33">
@@ -35297,7 +37195,7 @@
       <c r="B230" s="32">
         <v>80</v>
       </c>
-      <c r="C230" s="37" t="s">
+      <c r="C230" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D230" s="33">
@@ -35314,7 +37212,7 @@
       <c r="B231" s="32">
         <v>81</v>
       </c>
-      <c r="C231" s="37" t="s">
+      <c r="C231" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D231" s="33">
@@ -35331,7 +37229,7 @@
       <c r="B232" s="32">
         <v>82</v>
       </c>
-      <c r="C232" s="37" t="s">
+      <c r="C232" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D232" s="33">
@@ -35348,7 +37246,7 @@
       <c r="B233" s="32">
         <v>83</v>
       </c>
-      <c r="C233" s="37" t="s">
+      <c r="C233" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D233" s="33">
@@ -35365,7 +37263,7 @@
       <c r="B234" s="32">
         <v>84</v>
       </c>
-      <c r="C234" s="37" t="s">
+      <c r="C234" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D234" s="33">
@@ -35382,7 +37280,7 @@
       <c r="B235" s="32">
         <v>85</v>
       </c>
-      <c r="C235" s="37" t="s">
+      <c r="C235" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D235" s="33">
@@ -35399,7 +37297,7 @@
       <c r="B236" s="32">
         <v>86</v>
       </c>
-      <c r="C236" s="37" t="s">
+      <c r="C236" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D236" s="33">
@@ -35416,7 +37314,7 @@
       <c r="B237" s="32">
         <v>87</v>
       </c>
-      <c r="C237" s="37" t="s">
+      <c r="C237" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D237" s="33">
@@ -35433,7 +37331,7 @@
       <c r="B238" s="32">
         <v>88</v>
       </c>
-      <c r="C238" s="37" t="s">
+      <c r="C238" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D238" s="33">
@@ -35450,7 +37348,7 @@
       <c r="B239" s="32">
         <v>89</v>
       </c>
-      <c r="C239" s="37" t="s">
+      <c r="C239" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D239" s="33">
@@ -35467,7 +37365,7 @@
       <c r="B240" s="32">
         <v>90</v>
       </c>
-      <c r="C240" s="37" t="s">
+      <c r="C240" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D240" s="33">
@@ -35484,7 +37382,7 @@
       <c r="B241" s="32">
         <v>91</v>
       </c>
-      <c r="C241" s="37" t="s">
+      <c r="C241" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D241" s="33">
@@ -35501,7 +37399,7 @@
       <c r="B242" s="32">
         <v>92</v>
       </c>
-      <c r="C242" s="37" t="s">
+      <c r="C242" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D242" s="33">
@@ -35518,7 +37416,7 @@
       <c r="B243" s="32">
         <v>93</v>
       </c>
-      <c r="C243" s="37" t="s">
+      <c r="C243" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D243" s="33">
@@ -35535,7 +37433,7 @@
       <c r="B244" s="32">
         <v>94</v>
       </c>
-      <c r="C244" s="37" t="s">
+      <c r="C244" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D244" s="33">
@@ -35552,7 +37450,7 @@
       <c r="B245" s="32">
         <v>95</v>
       </c>
-      <c r="C245" s="37" t="s">
+      <c r="C245" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D245" s="33">
@@ -35569,7 +37467,7 @@
       <c r="B246" s="32">
         <v>96</v>
       </c>
-      <c r="C246" s="37" t="s">
+      <c r="C246" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D246" s="33">
@@ -35586,7 +37484,7 @@
       <c r="B247" s="32">
         <v>97</v>
       </c>
-      <c r="C247" s="37" t="s">
+      <c r="C247" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D247" s="33">
@@ -35603,7 +37501,7 @@
       <c r="B248" s="32">
         <v>98</v>
       </c>
-      <c r="C248" s="37" t="s">
+      <c r="C248" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D248" s="33">
@@ -35620,7 +37518,7 @@
       <c r="B249" s="32">
         <v>99</v>
       </c>
-      <c r="C249" s="37" t="s">
+      <c r="C249" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D249" s="33">
@@ -35637,7 +37535,7 @@
       <c r="B250" s="32">
         <v>100</v>
       </c>
-      <c r="C250" s="37" t="s">
+      <c r="C250" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D250" s="33">
@@ -35656,4 +37554,1113 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFBDAB2-974B-4516-AACB-B207FD61EF49}">
+  <dimension ref="A1:F85"/>
+  <sheetViews>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.3671875" customWidth="1"/>
+    <col min="3" max="3" width="11.15625" customWidth="1"/>
+    <col min="5" max="5" width="11.05078125" customWidth="1"/>
+    <col min="6" max="6" width="10.83984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="40">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40">
+        <v>18</v>
+      </c>
+      <c r="C3" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A3,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="40">
+        <v>1</v>
+      </c>
+      <c r="B4" s="40">
+        <v>19</v>
+      </c>
+      <c r="C4" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A4,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="40">
+        <v>1</v>
+      </c>
+      <c r="B5" s="40">
+        <v>20</v>
+      </c>
+      <c r="C5" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A5,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="40">
+        <v>1</v>
+      </c>
+      <c r="B6" s="40">
+        <v>21</v>
+      </c>
+      <c r="C6" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A6,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="40">
+        <v>1</v>
+      </c>
+      <c r="B7" s="40">
+        <v>22</v>
+      </c>
+      <c r="C7" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A7,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="40">
+        <v>1</v>
+      </c>
+      <c r="B8" s="40">
+        <v>23</v>
+      </c>
+      <c r="C8" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A8,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="40">
+        <v>1</v>
+      </c>
+      <c r="B9" s="40">
+        <v>24</v>
+      </c>
+      <c r="C9" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A9,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="40">
+        <v>1</v>
+      </c>
+      <c r="B10" s="40">
+        <v>25</v>
+      </c>
+      <c r="C10" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A10,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="40">
+        <v>1</v>
+      </c>
+      <c r="B11" s="40">
+        <v>26</v>
+      </c>
+      <c r="C11" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A11,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="40">
+        <v>1</v>
+      </c>
+      <c r="B12" s="40">
+        <v>27</v>
+      </c>
+      <c r="C12" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A12,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="40">
+        <v>1</v>
+      </c>
+      <c r="B13" s="40">
+        <v>28</v>
+      </c>
+      <c r="C13" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A13,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="40">
+        <v>1</v>
+      </c>
+      <c r="B14" s="40">
+        <v>29</v>
+      </c>
+      <c r="C14" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A14,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="40">
+        <v>1</v>
+      </c>
+      <c r="B15" s="40">
+        <v>30</v>
+      </c>
+      <c r="C15" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A15,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="40">
+        <v>1</v>
+      </c>
+      <c r="B16" s="40">
+        <v>31</v>
+      </c>
+      <c r="C16" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A16,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="40">
+        <v>1</v>
+      </c>
+      <c r="B17" s="40">
+        <v>32</v>
+      </c>
+      <c r="C17" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A17,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="40">
+        <v>1</v>
+      </c>
+      <c r="B18" s="40">
+        <v>33</v>
+      </c>
+      <c r="C18" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A18,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="40">
+        <v>1</v>
+      </c>
+      <c r="B19" s="40">
+        <v>34</v>
+      </c>
+      <c r="C19" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A19,Table413[],2)</f>
+        <v>18-34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="40">
+        <v>2</v>
+      </c>
+      <c r="B20" s="40">
+        <v>35</v>
+      </c>
+      <c r="C20" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A20,Table413[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="40">
+        <v>2</v>
+      </c>
+      <c r="B21" s="40">
+        <v>36</v>
+      </c>
+      <c r="C21" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A21,Table413[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="40">
+        <v>2</v>
+      </c>
+      <c r="B22" s="40">
+        <v>37</v>
+      </c>
+      <c r="C22" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A22,Table413[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="40">
+        <v>2</v>
+      </c>
+      <c r="B23" s="40">
+        <v>38</v>
+      </c>
+      <c r="C23" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A23,Table413[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="40">
+        <v>2</v>
+      </c>
+      <c r="B24" s="40">
+        <v>39</v>
+      </c>
+      <c r="C24" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A24,Table413[],2)</f>
+        <v>35-39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="40">
+        <v>3</v>
+      </c>
+      <c r="B25" s="40">
+        <v>40</v>
+      </c>
+      <c r="C25" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A25,Table413[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="40">
+        <v>3</v>
+      </c>
+      <c r="B26" s="40">
+        <v>41</v>
+      </c>
+      <c r="C26" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A26,Table413[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="40">
+        <v>3</v>
+      </c>
+      <c r="B27" s="40">
+        <v>42</v>
+      </c>
+      <c r="C27" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A27,Table413[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="40">
+        <v>3</v>
+      </c>
+      <c r="B28" s="40">
+        <v>43</v>
+      </c>
+      <c r="C28" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A28,Table413[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="40">
+        <v>3</v>
+      </c>
+      <c r="B29" s="40">
+        <v>44</v>
+      </c>
+      <c r="C29" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A29,Table413[],2)</f>
+        <v>40-44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="40">
+        <v>4</v>
+      </c>
+      <c r="B30" s="40">
+        <v>45</v>
+      </c>
+      <c r="C30" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A30,Table413[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="40">
+        <v>4</v>
+      </c>
+      <c r="B31" s="40">
+        <v>46</v>
+      </c>
+      <c r="C31" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A31,Table413[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="40">
+        <v>4</v>
+      </c>
+      <c r="B32" s="40">
+        <v>47</v>
+      </c>
+      <c r="C32" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A32,Table413[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="40">
+        <v>4</v>
+      </c>
+      <c r="B33" s="40">
+        <v>48</v>
+      </c>
+      <c r="C33" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A33,Table413[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="40">
+        <v>4</v>
+      </c>
+      <c r="B34" s="40">
+        <v>49</v>
+      </c>
+      <c r="C34" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A34,Table413[],2)</f>
+        <v>45-49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="40">
+        <v>5</v>
+      </c>
+      <c r="B35" s="40">
+        <v>50</v>
+      </c>
+      <c r="C35" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A35,Table413[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="40">
+        <v>5</v>
+      </c>
+      <c r="B36" s="40">
+        <v>51</v>
+      </c>
+      <c r="C36" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A36,Table413[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="40">
+        <v>5</v>
+      </c>
+      <c r="B37" s="40">
+        <v>52</v>
+      </c>
+      <c r="C37" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A37,Table413[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="40">
+        <v>5</v>
+      </c>
+      <c r="B38" s="40">
+        <v>53</v>
+      </c>
+      <c r="C38" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A38,Table413[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="40">
+        <v>5</v>
+      </c>
+      <c r="B39" s="40">
+        <v>54</v>
+      </c>
+      <c r="C39" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A39,Table413[],2)</f>
+        <v>50-54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="40">
+        <v>6</v>
+      </c>
+      <c r="B40" s="40">
+        <v>55</v>
+      </c>
+      <c r="C40" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A40,Table413[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="40">
+        <v>6</v>
+      </c>
+      <c r="B41" s="40">
+        <v>56</v>
+      </c>
+      <c r="C41" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A41,Table413[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="40">
+        <v>6</v>
+      </c>
+      <c r="B42" s="40">
+        <v>57</v>
+      </c>
+      <c r="C42" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A42,Table413[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="40">
+        <v>6</v>
+      </c>
+      <c r="B43" s="40">
+        <v>58</v>
+      </c>
+      <c r="C43" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A43,Table413[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="40">
+        <v>6</v>
+      </c>
+      <c r="B44" s="40">
+        <v>59</v>
+      </c>
+      <c r="C44" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A44,Table413[],2)</f>
+        <v>55-59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="40">
+        <v>7</v>
+      </c>
+      <c r="B45" s="40">
+        <v>60</v>
+      </c>
+      <c r="C45" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A45,Table413[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="40">
+        <v>7</v>
+      </c>
+      <c r="B46" s="40">
+        <v>61</v>
+      </c>
+      <c r="C46" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A46,Table413[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="40">
+        <v>7</v>
+      </c>
+      <c r="B47" s="40">
+        <v>62</v>
+      </c>
+      <c r="C47" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A47,Table413[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="40">
+        <v>7</v>
+      </c>
+      <c r="B48" s="40">
+        <v>63</v>
+      </c>
+      <c r="C48" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A48,Table413[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="40">
+        <v>7</v>
+      </c>
+      <c r="B49" s="40">
+        <v>64</v>
+      </c>
+      <c r="C49" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A49,Table413[],2)</f>
+        <v>60-64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="40">
+        <v>8</v>
+      </c>
+      <c r="B50" s="40">
+        <v>65</v>
+      </c>
+      <c r="C50" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A50,Table413[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="40">
+        <v>8</v>
+      </c>
+      <c r="B51" s="40">
+        <v>66</v>
+      </c>
+      <c r="C51" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A51,Table413[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="40">
+        <v>8</v>
+      </c>
+      <c r="B52" s="40">
+        <v>67</v>
+      </c>
+      <c r="C52" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A52,Table413[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="40">
+        <v>8</v>
+      </c>
+      <c r="B53" s="40">
+        <v>68</v>
+      </c>
+      <c r="C53" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A53,Table413[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="40">
+        <v>8</v>
+      </c>
+      <c r="B54" s="40">
+        <v>69</v>
+      </c>
+      <c r="C54" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A54,Table413[],2)</f>
+        <v>65-69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="40">
+        <v>9</v>
+      </c>
+      <c r="B55" s="40">
+        <v>70</v>
+      </c>
+      <c r="C55" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A55,Table413[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="40">
+        <v>9</v>
+      </c>
+      <c r="B56" s="40">
+        <v>71</v>
+      </c>
+      <c r="C56" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A56,Table413[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="40">
+        <v>9</v>
+      </c>
+      <c r="B57" s="40">
+        <v>72</v>
+      </c>
+      <c r="C57" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A57,Table413[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="40">
+        <v>9</v>
+      </c>
+      <c r="B58" s="40">
+        <v>73</v>
+      </c>
+      <c r="C58" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A58,Table413[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="40">
+        <v>9</v>
+      </c>
+      <c r="B59" s="40">
+        <v>74</v>
+      </c>
+      <c r="C59" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A59,Table413[],2)</f>
+        <v>70-74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="40">
+        <v>10</v>
+      </c>
+      <c r="B60" s="40">
+        <v>75</v>
+      </c>
+      <c r="C60" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A60,Table413[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="40">
+        <v>10</v>
+      </c>
+      <c r="B61" s="40">
+        <v>76</v>
+      </c>
+      <c r="C61" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A61,Table413[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="40">
+        <v>10</v>
+      </c>
+      <c r="B62" s="40">
+        <v>77</v>
+      </c>
+      <c r="C62" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A62,Table413[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="40">
+        <v>10</v>
+      </c>
+      <c r="B63" s="40">
+        <v>78</v>
+      </c>
+      <c r="C63" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A63,Table413[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="40">
+        <v>10</v>
+      </c>
+      <c r="B64" s="40">
+        <v>79</v>
+      </c>
+      <c r="C64" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A64,Table413[],2)</f>
+        <v>75-79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="40">
+        <v>11</v>
+      </c>
+      <c r="B65" s="40">
+        <v>80</v>
+      </c>
+      <c r="C65" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A65,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="40">
+        <v>11</v>
+      </c>
+      <c r="B66" s="40">
+        <v>81</v>
+      </c>
+      <c r="C66" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A66,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="40">
+        <v>11</v>
+      </c>
+      <c r="B67" s="40">
+        <v>82</v>
+      </c>
+      <c r="C67" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A67,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="40">
+        <v>11</v>
+      </c>
+      <c r="B68" s="40">
+        <v>83</v>
+      </c>
+      <c r="C68" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A68,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="40">
+        <v>11</v>
+      </c>
+      <c r="B69" s="40">
+        <v>84</v>
+      </c>
+      <c r="C69" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A69,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="40">
+        <v>11</v>
+      </c>
+      <c r="B70" s="40">
+        <v>85</v>
+      </c>
+      <c r="C70" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A70,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="40">
+        <v>11</v>
+      </c>
+      <c r="B71" s="40">
+        <v>86</v>
+      </c>
+      <c r="C71" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A71,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="40">
+        <v>11</v>
+      </c>
+      <c r="B72" s="40">
+        <v>87</v>
+      </c>
+      <c r="C72" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A72,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="40">
+        <v>11</v>
+      </c>
+      <c r="B73" s="40">
+        <v>88</v>
+      </c>
+      <c r="C73" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A73,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="40">
+        <v>11</v>
+      </c>
+      <c r="B74" s="40">
+        <v>89</v>
+      </c>
+      <c r="C74" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A74,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="40">
+        <v>11</v>
+      </c>
+      <c r="B75" s="40">
+        <v>90</v>
+      </c>
+      <c r="C75" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A75,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="40">
+        <v>11</v>
+      </c>
+      <c r="B76" s="40">
+        <v>91</v>
+      </c>
+      <c r="C76" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A76,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="40">
+        <v>11</v>
+      </c>
+      <c r="B77" s="40">
+        <v>92</v>
+      </c>
+      <c r="C77" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A77,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="40">
+        <v>11</v>
+      </c>
+      <c r="B78" s="40">
+        <v>93</v>
+      </c>
+      <c r="C78" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A78,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="40">
+        <v>11</v>
+      </c>
+      <c r="B79" s="40">
+        <v>94</v>
+      </c>
+      <c r="C79" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A79,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="40">
+        <v>11</v>
+      </c>
+      <c r="B80" s="40">
+        <v>95</v>
+      </c>
+      <c r="C80" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A80,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="40">
+        <v>11</v>
+      </c>
+      <c r="B81" s="40">
+        <v>96</v>
+      </c>
+      <c r="C81" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A81,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="40">
+        <v>11</v>
+      </c>
+      <c r="B82" s="40">
+        <v>97</v>
+      </c>
+      <c r="C82" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A82,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="40">
+        <v>11</v>
+      </c>
+      <c r="B83" s="40">
+        <v>98</v>
+      </c>
+      <c r="C83" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A83,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="40">
+        <v>11</v>
+      </c>
+      <c r="B84" s="40">
+        <v>99</v>
+      </c>
+      <c r="C84" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A84,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="40">
+        <v>11</v>
+      </c>
+      <c r="B85" s="40">
+        <v>100</v>
+      </c>
+      <c r="C85" s="41" t="str">
+        <f>VLOOKUP([1]Bos_Age_Groups!$A85,Table413[],2)</f>
+        <v>80+</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>